<commit_message>
memperbaiki indomaret poshop merdeka
</commit_message>
<xml_diff>
--- a/indomaretv3/df_merged_repaired.xlsx
+++ b/indomaretv3/df_merged_repaired.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpram\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4204839E-146A-4AAC-8627-228FFF4B5063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8994D3-5940-4E9F-B1E0-CBCE26ECE3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2374,8 +2374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C272" zoomScale="91" workbookViewId="0">
-      <selection activeCell="H334" sqref="H334"/>
+    <sheetView tabSelected="1" topLeftCell="H201" zoomScale="91" workbookViewId="0">
+      <selection activeCell="H212" sqref="H212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8498,16 +8498,16 @@
         <v>104.75987670000001</v>
       </c>
       <c r="F211" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="G211" t="s">
         <v>422</v>
       </c>
       <c r="H211" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="I211">
-        <v>1689</v>
+        <v>16048</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>